<commit_message>
Common: Another set of data for import
</commit_message>
<xml_diff>
--- a/fixtures/02 - vendors.xlsx
+++ b/fixtures/02 - vendors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127E4D9E-D97A-4D43-86B1-A84D3DF846E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01D1C06-AFF4-406E-9E35-35D8BE385B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="1725" windowWidth="23610" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1095" yWindow="2160" windowWidth="23610" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>tab</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>KeepPower</t>
+  </si>
+  <si>
+    <t>Rocket Girl</t>
   </si>
 </sst>
 </file>
@@ -704,10 +707,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AEBD79-8DB9-48DF-B83D-337964022B0C}">
-  <dimension ref="A1:A95"/>
+  <dimension ref="A1:A96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,172 +1030,177 @@
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A95">
-    <sortCondition ref="A94:A95"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A96">
+    <sortCondition ref="A90:A96"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>